<commit_message>
refined Ante and Started Adding in Some skills for testing
</commit_message>
<xml_diff>
--- a/Strix_Take_3/Planning/Skills.xlsx
+++ b/Strix_Take_3/Planning/Skills.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McKay\Desktop\Strixhaven\Strixhaven_RPG_Project\Strix_Take_3\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pengu\Desktop\Strix Take 3, For Real\Strix_Take_3\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1FEA23-3802-475B-85E6-35770AA6398F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DDA561-B756-4F57-A83B-2870CFB4C204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31860" yWindow="6345" windowWidth="20910" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Statuss" sheetId="3" r:id="rId1"/>
+    <sheet name="Status Ef" sheetId="3" r:id="rId1"/>
     <sheet name="Javenesh" sheetId="1" r:id="rId2"/>
     <sheet name="Tilana" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="84">
   <si>
     <t>Skill Name</t>
   </si>
@@ -128,31 +128,157 @@
     <t>Crashing Desent</t>
   </si>
   <si>
-    <t>Untility</t>
-  </si>
-  <si>
     <t>40 + (2 * Ante)</t>
   </si>
   <si>
     <t>(Ante set: 0)</t>
   </si>
   <si>
-    <t>Blinding Strike</t>
-  </si>
-  <si>
-    <t>Utility</t>
-  </si>
-  <si>
     <t>Blunt</t>
   </si>
   <si>
-    <t>(Forces next Ante: Attack)</t>
-  </si>
-  <si>
     <t>Force Dart</t>
   </si>
   <si>
     <t>Card Spray</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Debuff</t>
+  </si>
+  <si>
+    <t>Multi</t>
+  </si>
+  <si>
+    <t>(-25% Accuracy) (+15% Crit Taken Chance)</t>
+  </si>
+  <si>
+    <t>Blinded</t>
+  </si>
+  <si>
+    <t>(40%)(Blinded)(3 Turns)</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>Frostbite</t>
+  </si>
+  <si>
+    <t>Riptide</t>
+  </si>
+  <si>
+    <t>Stat Up/Down</t>
+  </si>
+  <si>
+    <t>(-15% to Stat per Level) (3 Stacks Max)</t>
+  </si>
+  <si>
+    <t>(-20% Speed) (-10% Evasion)</t>
+  </si>
+  <si>
+    <t>(Forces Target Down 1 in Turn order, Current and Next)(Speed Down 3 Turns)</t>
+  </si>
+  <si>
+    <t>Magic Daggers</t>
+  </si>
+  <si>
+    <t>Spread</t>
+  </si>
+  <si>
+    <t>(50%)(Bleed)(3 Turns)</t>
+  </si>
+  <si>
+    <t>Bleed</t>
+  </si>
+  <si>
+    <t>(-5% Hp Regen)(-15% Strength)(-15% Defense)</t>
+  </si>
+  <si>
+    <t>Clear Winds</t>
+  </si>
+  <si>
+    <t>(Clears Stat Downs) (+5% Hp Regen)(3 Turns)</t>
+  </si>
+  <si>
+    <t>Magic Missle</t>
+  </si>
+  <si>
+    <t>5 (6 Times)</t>
+  </si>
+  <si>
+    <t>Gambit</t>
+  </si>
+  <si>
+    <t>Leading Strike</t>
+  </si>
+  <si>
+    <t>(Forces Next Ante Draw: Attack)</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>(-50% Def &amp; M. Def)(+100% Atk)(Provoke on random Enemy) (1 Turn) (+ 3 Ante) (5 Cooldown)</t>
+  </si>
+  <si>
+    <t>Witch Bolt</t>
+  </si>
+  <si>
+    <t>Static</t>
+  </si>
+  <si>
+    <t>(-5% Hp Regen)(-15% Magic)(-15% M.Def)</t>
+  </si>
+  <si>
+    <t>(70%)(Static)(3 Turns)</t>
+  </si>
+  <si>
+    <t>(Allways Hits)(%2.5 chance to add Blinded/Bleed/Static)(3 Turns)</t>
+  </si>
+  <si>
+    <t>Ray of Enfeblement</t>
+  </si>
+  <si>
+    <t>Acid</t>
+  </si>
+  <si>
+    <t>Acid Splash</t>
+  </si>
+  <si>
+    <t>Eldritch Orb</t>
+  </si>
+  <si>
+    <t>(%5 chance to add Blinded/Bleed/Static)(3 Turns)</t>
+  </si>
+  <si>
+    <t>(Speed &amp; Def &amp; M.Def Down)(2 Stages)(3 Turns)</t>
+  </si>
+  <si>
+    <t>(All Stats Down 1 Stage)(5 Turns)</t>
+  </si>
+  <si>
+    <t>(Def and M.Def Down 2 Stages)(3 Turns)</t>
+  </si>
+  <si>
+    <t>Phys/Mag</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Magical</t>
+  </si>
+  <si>
+    <t>Buff</t>
+  </si>
+  <si>
+    <t>Necrotic</t>
   </si>
 </sst>
 </file>
@@ -470,34 +596,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04557686-FCB8-4071-B6C9-CFD73AFC9DC4}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="66.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.73046875" customWidth="1"/>
-    <col min="2" max="2" width="11.59765625" customWidth="1"/>
-    <col min="6" max="6" width="14.1328125" customWidth="1"/>
-    <col min="7" max="7" width="13.1328125" customWidth="1"/>
-    <col min="8" max="8" width="59.3984375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,22 +690,25 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -534,22 +719,25 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>22</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>20</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>95</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -560,22 +748,25 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -586,19 +777,22 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>30</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -609,22 +803,25 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>10</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>100</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -632,25 +829,28 @@
         <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>21</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>27</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -661,19 +861,22 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>24</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>30</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -684,22 +887,25 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>20</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>27</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -710,45 +916,109 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>22</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9">
+        <v>95</v>
+      </c>
+      <c r="I9" t="s">
         <v>34</v>
       </c>
-      <c r="G9">
-        <v>95</v>
-      </c>
-      <c r="H9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="B10">
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
         <v>22</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>30</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>90</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
         <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11">
+        <v>25</v>
+      </c>
+      <c r="H11">
+        <v>90</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>100</v>
+      </c>
+      <c r="I12" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -758,19 +1028,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC2511E-84A4-45C1-858A-C7C6F6DE91AF}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" customWidth="1"/>
-    <col min="6" max="6" width="16.06640625" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="8" max="8" width="106.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -796,7 +1067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -807,7 +1078,7 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -822,7 +1093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -848,14 +1119,261 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>41</v>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>90</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
+      </c>
+      <c r="G6">
+        <v>90</v>
+      </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>95</v>
+      </c>
+      <c r="H9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+      <c r="G10">
+        <v>95</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11">
+        <v>30</v>
+      </c>
+      <c r="G11">
+        <v>95</v>
+      </c>
+      <c r="H11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>90</v>
+      </c>
+      <c r="H12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13">
+        <v>40</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the Damage Calc and Started Lil's Skills
</commit_message>
<xml_diff>
--- a/Strix_Take_3/Planning/Skills.xlsx
+++ b/Strix_Take_3/Planning/Skills.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pengu\Desktop\Strix Take 3, For Real\Strix_Take_3\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DDA561-B756-4F57-A83B-2870CFB4C204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3405FEA4-6349-4B09-9DC1-E384E782A2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31860" yWindow="6345" windowWidth="20910" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Status Ef" sheetId="3" r:id="rId1"/>
-    <sheet name="Javenesh" sheetId="1" r:id="rId2"/>
-    <sheet name="Tilana" sheetId="2" r:id="rId3"/>
+    <sheet name="Damage Calc" sheetId="6" r:id="rId1"/>
+    <sheet name="Status Ef" sheetId="3" r:id="rId2"/>
+    <sheet name="Javenesh" sheetId="1" r:id="rId3"/>
+    <sheet name="Tilana" sheetId="2" r:id="rId4"/>
+    <sheet name="Gorjsh" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="110">
   <si>
     <t>Skill Name</t>
   </si>
@@ -194,9 +197,6 @@
     <t>Bleed</t>
   </si>
   <si>
-    <t>(-5% Hp Regen)(-15% Strength)(-15% Defense)</t>
-  </si>
-  <si>
     <t>Clear Winds</t>
   </si>
   <si>
@@ -233,9 +233,6 @@
     <t>Static</t>
   </si>
   <si>
-    <t>(-5% Hp Regen)(-15% Magic)(-15% M.Def)</t>
-  </si>
-  <si>
     <t>(70%)(Static)(3 Turns)</t>
   </si>
   <si>
@@ -279,6 +276,90 @@
   </si>
   <si>
     <t>Necrotic</t>
+  </si>
+  <si>
+    <t>Poison Bubble</t>
+  </si>
+  <si>
+    <t>Mag</t>
+  </si>
+  <si>
+    <t>(80%)(Poison)(3 Turns)</t>
+  </si>
+  <si>
+    <t>(-(User Atk/M.Atk) Hp Regen)(-15% Strength)(-15% Defense)</t>
+  </si>
+  <si>
+    <t>(-(User Atk/M.Atk) Hp Regen)(-15% Magic)(-15% M.Def)</t>
+  </si>
+  <si>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>(-(User Atk/M.Atk * 2) Hp Regen)</t>
+  </si>
+  <si>
+    <t>Healing Cauldron</t>
+  </si>
+  <si>
+    <t>Healing Brew</t>
+  </si>
+  <si>
+    <t>Bitter Brew</t>
+  </si>
+  <si>
+    <t>(Clears Status Effects)</t>
+  </si>
+  <si>
+    <t>Critical Brew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(+25% Crit Up)(3 Turns) </t>
+  </si>
+  <si>
+    <t>Rusting Vials</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>5 * (5)</t>
+  </si>
+  <si>
+    <t>(40%)(Def Down), (30%)(Atk Down)</t>
+  </si>
+  <si>
+    <t>Flair Vials</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>(40%)(M.Def Down), (30%)(M.Atk Down)</t>
+  </si>
+  <si>
+    <t>Invigerating Cauldron</t>
+  </si>
+  <si>
+    <t>(All Stats up)(3 Turns)</t>
+  </si>
+  <si>
+    <t>Acid Arrow</t>
+  </si>
+  <si>
+    <t>(50% M.Def Pierce)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poison Fog </t>
+  </si>
+  <si>
+    <t>(70%)(Posion)(3 Turns)</t>
+  </si>
+  <si>
+    <t>Empty Vials</t>
+  </si>
+  <si>
+    <t>((Atk Stat / 2) * (Base Damage)) / (Def Stat / 2)</t>
   </si>
 </sst>
 </file>
@@ -595,11 +676,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F0069A-5567-4FAA-90C8-D98F947CC81F}">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04557686-FCB8-4071-B6C9-CFD73AFC9DC4}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,15 +749,23 @@
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -661,12 +773,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +802,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -719,7 +831,7 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -777,7 +889,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -803,7 +915,7 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -829,10 +941,10 @@
         <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -861,7 +973,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -887,7 +999,7 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -916,7 +1028,7 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E9" t="s">
         <v>17</v>
@@ -936,7 +1048,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10">
         <v>20</v>
@@ -945,7 +1057,7 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s">
         <v>35</v>
@@ -960,7 +1072,7 @@
         <v>90</v>
       </c>
       <c r="I10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -974,7 +1086,7 @@
         <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
         <v>35</v>
@@ -994,7 +1106,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12">
         <v>25</v>
@@ -1003,7 +1115,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
         <v>3</v>
@@ -1018,7 +1130,7 @@
         <v>100</v>
       </c>
       <c r="I12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1026,12 +1138,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC2511E-84A4-45C1-858A-C7C6F6DE91AF}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,7 +1262,7 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -1176,7 +1288,7 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -1196,7 +1308,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -1211,18 +1323,18 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G7" t="s">
         <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1243,12 +1355,12 @@
         <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9">
         <v>30</v>
@@ -1269,18 +1381,18 @@
         <v>95</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10">
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -1295,12 +1407,12 @@
         <v>95</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11">
         <v>30</v>
@@ -1309,7 +1421,7 @@
         <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
@@ -1321,12 +1433,12 @@
         <v>95</v>
       </c>
       <c r="H11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12">
         <v>35</v>
@@ -1335,7 +1447,7 @@
         <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E12" t="s">
         <v>40</v>
@@ -1347,12 +1459,12 @@
         <v>90</v>
       </c>
       <c r="H12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B13">
         <v>50</v>
@@ -1373,7 +1485,452 @@
         <v>100</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6313457-33D7-4830-B1BD-E1AB874C1CA0}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
+    <col min="9" max="9" width="86.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>95</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>95</v>
+      </c>
+      <c r="I4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>100</v>
+      </c>
+      <c r="I8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9">
+        <v>85</v>
+      </c>
+      <c r="I9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10">
+        <v>85</v>
+      </c>
+      <c r="I10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+      <c r="I11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12">
+        <v>35</v>
+      </c>
+      <c r="H12">
+        <v>95</v>
+      </c>
+      <c r="I12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>100</v>
+      </c>
+      <c r="I13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A481FDDE-6AFA-4D67-BC7D-7FCADA58E53C}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="90.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>